<commit_message>
Update only central LMS scenarios; copy and paste central pension mobility to short-term globals for central mobility, after Detailed_Anses_Income_V3; must be recomputed to include endogenous elements of the model (ANSES contributions and total beneficiaries).
</commit_message>
<xml_diff>
--- a/Excel_files_for_MISSAR/Prospective_scenarios/2014_q4_start/Historical_graphs_ages_16_69/Economic_scenarios_representation_nov_2020.xlsx
+++ b/Excel_files_for_MISSAR/Prospective_scenarios/2014_q4_start/Historical_graphs_ages_16_69/Economic_scenarios_representation_nov_2020.xlsx
@@ -841,7 +841,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart55.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart57.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -21052,11 +21052,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="74846718"/>
-        <c:axId val="3920625"/>
+        <c:axId val="68638324"/>
+        <c:axId val="71095290"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="74846718"/>
+        <c:axId val="68638324"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21088,14 +21088,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3920625"/>
+        <c:crossAx val="71095290"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="3920625"/>
+        <c:axId val="71095290"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.8"/>
@@ -21138,7 +21138,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74846718"/>
+        <c:crossAx val="68638324"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -21202,7 +21202,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart56.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart58.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -31139,7 +31139,7 @@
                   <c:v>0.125</c:v>
                 </c:pt>
                 <c:pt idx="183">
-                  <c:v>0.1523</c:v>
+                  <c:v>0.1423</c:v>
                 </c:pt>
                 <c:pt idx="184">
                   <c:v>0.1475</c:v>
@@ -40109,7 +40109,7 @@
                   <c:v>0.5237</c:v>
                 </c:pt>
                 <c:pt idx="183">
-                  <c:v>0.49</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="184">
                   <c:v>0.47</c:v>
@@ -41450,11 +41450,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="20189086"/>
-        <c:axId val="61333473"/>
+        <c:axId val="35159912"/>
+        <c:axId val="39037296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="20189086"/>
+        <c:axId val="35159912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -41486,14 +41486,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61333473"/>
+        <c:crossAx val="39037296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="61333473"/>
+        <c:axId val="39037296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.8"/>
@@ -41537,7 +41537,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20189086"/>
+        <c:crossAx val="35159912"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -41605,14 +41605,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>61</xdr:col>
-      <xdr:colOff>604440</xdr:colOff>
+      <xdr:col>64</xdr:col>
+      <xdr:colOff>385920</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>98</xdr:col>
-      <xdr:colOff>59760</xdr:colOff>
+      <xdr:col>100</xdr:col>
+      <xdr:colOff>474480</xdr:colOff>
       <xdr:row>70</xdr:row>
       <xdr:rowOff>122040</xdr:rowOff>
     </xdr:to>
@@ -41622,7 +41622,7 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="39165840" y="0"/>
+        <a:off x="40846680" y="0"/>
         <a:ext cx="22879800" cy="10789920"/>
       </xdr:xfrm>
       <a:graphic>
@@ -41635,16 +41635,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>45</xdr:col>
-      <xdr:colOff>424440</xdr:colOff>
-      <xdr:row>86</xdr:row>
-      <xdr:rowOff>117720</xdr:rowOff>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>628560</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>109800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>81</xdr:col>
-      <xdr:colOff>459360</xdr:colOff>
-      <xdr:row>157</xdr:row>
-      <xdr:rowOff>100440</xdr:rowOff>
+      <xdr:col>83</xdr:col>
+      <xdr:colOff>30240</xdr:colOff>
+      <xdr:row>155</xdr:row>
+      <xdr:rowOff>92880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -41652,7 +41652,7 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="28856520" y="13223880"/>
+        <a:off x="29693520" y="12911400"/>
         <a:ext cx="22826160" cy="10803240"/>
       </xdr:xfrm>
       <a:graphic>
@@ -41799,8 +41799,8 @@
   </sheetPr>
   <dimension ref="A1:BL284"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S159" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AG194" activeCellId="0" sqref="AG194"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AD147" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AR192" activeCellId="0" sqref="AR192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -54831,7 +54831,7 @@
       </c>
       <c r="BG175" s="1" t="n">
         <f aca="false">(AR190-AM185)/(ROW(AR190)-ROW(AM185))</f>
-        <v>-0.00996506827999998</v>
+        <v>-0.01196506828</v>
       </c>
       <c r="BH175" s="0" t="n">
         <f aca="false">(AS190-AN185)/(ROW(AS190)-ROW(AN185))</f>
@@ -54839,7 +54839,7 @@
       </c>
       <c r="BI175" s="1" t="n">
         <f aca="false">(AT190-AO185)/(ROW(AT190)-ROW(AO185))</f>
-        <v>0.01545988058</v>
+        <v>0.01745988058</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -55670,7 +55670,7 @@
       </c>
       <c r="BG183" s="5" t="n">
         <f aca="false">AR190+$AB$175</f>
-        <v>0.128989816675</v>
+        <v>0.118989816675</v>
       </c>
       <c r="BH183" s="1" t="n">
         <f aca="false">AS190+$AC$175</f>
@@ -55678,7 +55678,7 @@
       </c>
       <c r="BI183" s="1" t="n">
         <f aca="false">AT190+$AD$175</f>
-        <v>0.520810658925</v>
+        <v>0.530810658925</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -56300,13 +56300,13 @@
       </c>
       <c r="AR190" s="5" t="n">
         <f aca="false">1-(AP190+AQ190+AT190+AS190)</f>
-        <v>0.1523</v>
+        <v>0.1423</v>
       </c>
       <c r="AS190" s="5" t="n">
         <v>0.065</v>
       </c>
       <c r="AT190" s="5" t="n">
-        <v>0.49</v>
+        <v>0.5</v>
       </c>
       <c r="AU190" s="8"/>
       <c r="AV190" s="8"/>

</xml_diff>

<commit_message>
Correct error on LMS alignment tables: not properly reflected EPH 2d quarter 2020 on prospective tables
</commit_message>
<xml_diff>
--- a/Excel_files_for_MISSAR/Prospective_scenarios/2014_q4_start/Historical_graphs_ages_16_69/Economic_scenarios_representation_nov_2020.xlsx
+++ b/Excel_files_for_MISSAR/Prospective_scenarios/2014_q4_start/Historical_graphs_ages_16_69/Economic_scenarios_representation_nov_2020.xlsx
@@ -841,7 +841,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart57.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart71.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -852,10 +852,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0524891434325634"/>
-          <c:y val="0.0202849230974544"/>
-          <c:w val="0.917348480080559"/>
-          <c:h val="0.62549627998532"/>
+          <c:x val="0.0524843207217969"/>
+          <c:y val="0.0202855998932337"/>
+          <c:w val="0.917336015970072"/>
+          <c:h val="0.625483784865875"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -866,7 +866,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$6</c:f>
+              <c:f>Sheet1!$F$6:$F$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2051,7 +2051,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$P$6</c:f>
+              <c:f>Sheet1!$P$6:$P$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3140,7 +3140,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$K$6</c:f>
+              <c:f>Sheet1!$K$6:$K$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4244,7 +4244,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$T$6</c:f>
+              <c:f>Sheet1!$T$6:$T$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5333,7 +5333,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$6</c:f>
+              <c:f>Sheet1!$G$6:$G$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6521,7 +6521,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$L$6</c:f>
+              <c:f>Sheet1!$L$6:$L$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7625,7 +7625,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$6</c:f>
+              <c:f>Sheet1!$H$6:$H$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8810,7 +8810,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Q$6</c:f>
+              <c:f>Sheet1!$Q$6:$Q$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -9899,7 +9899,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$M$6</c:f>
+              <c:f>Sheet1!$M$6:$M$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -11003,7 +11003,7 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$U$6</c:f>
+              <c:f>Sheet1!$U$6:$U$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -12092,7 +12092,7 @@
           <c:order val="10"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$I$6</c:f>
+              <c:f>Sheet1!$I$6:$I$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -13277,7 +13277,7 @@
           <c:order val="11"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$R$6</c:f>
+              <c:f>Sheet1!$R$6:$R$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -14370,7 +14370,7 @@
           <c:order val="12"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$N$6</c:f>
+              <c:f>Sheet1!$N$6:$N$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -15478,7 +15478,7 @@
           <c:order val="13"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$V$6</c:f>
+              <c:f>Sheet1!$V$6:$V$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -16567,7 +16567,7 @@
           <c:order val="14"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$J$6</c:f>
+              <c:f>Sheet1!$J$6:$J$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -17767,7 +17767,7 @@
           <c:order val="15"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$S$6</c:f>
+              <c:f>Sheet1!$S$6:$S$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -18856,7 +18856,7 @@
           <c:order val="16"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$O$6</c:f>
+              <c:f>Sheet1!$O$6:$O$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -19960,7 +19960,7 @@
           <c:order val="17"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$W$6</c:f>
+              <c:f>Sheet1!$W$6:$W$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -21052,11 +21052,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="68638324"/>
-        <c:axId val="71095290"/>
+        <c:axId val="13657991"/>
+        <c:axId val="14739751"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="68638324"/>
+        <c:axId val="13657991"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21088,14 +21088,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71095290"/>
+        <c:crossAx val="14739751"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71095290"/>
+        <c:axId val="14739751"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.8"/>
@@ -21138,7 +21138,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68638324"/>
+        <c:crossAx val="13657991"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -21202,7 +21202,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart58.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart72.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -21213,10 +21213,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0465090605138234"/>
-          <c:y val="0.0268243918693769"/>
-          <c:w val="0.940795180342864"/>
-          <c:h val="0.590936354548484"/>
+          <c:x val="0.0465094295032377"/>
+          <c:y val="0.0268252857476091"/>
+          <c:w val="0.940776102471995"/>
+          <c:h val="0.590922723183045"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -21227,7 +21227,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AK$6</c:f>
+              <c:f>Sheet1!$AK$6:$AK$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -22415,7 +22415,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AU$6</c:f>
+              <c:f>Sheet1!$AU$6:$AU$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -23507,7 +23507,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AP$6</c:f>
+              <c:f>Sheet1!$AP$6:$AP$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -24614,7 +24614,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AY$6</c:f>
+              <c:f>Sheet1!$AY$6:$AY$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -25706,7 +25706,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AL$6</c:f>
+              <c:f>Sheet1!$AL$6:$AL$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -26894,7 +26894,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AQ$6</c:f>
+              <c:f>Sheet1!$AQ$6:$AQ$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -28001,7 +28001,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AM$6</c:f>
+              <c:f>Sheet1!$AM$6:$AM$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -29186,7 +29186,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AV$6</c:f>
+              <c:f>Sheet1!$AV$6:$AV$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -30278,7 +30278,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AR$6</c:f>
+              <c:f>Sheet1!$AR$6:$AR$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -31385,7 +31385,7 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AZ$6</c:f>
+              <c:f>Sheet1!$AZ$6:$AZ$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -32477,7 +32477,7 @@
           <c:order val="10"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AN$6</c:f>
+              <c:f>Sheet1!$AN$6:$AN$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -33662,7 +33662,7 @@
           <c:order val="11"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AW$6</c:f>
+              <c:f>Sheet1!$AW$6:$AW$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -34754,7 +34754,7 @@
           <c:order val="12"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AS$6</c:f>
+              <c:f>Sheet1!$AS$6:$AS$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -35861,7 +35861,7 @@
           <c:order val="13"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$BA$6</c:f>
+              <c:f>Sheet1!$BA$6:$BA$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -36953,7 +36953,7 @@
           <c:order val="14"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AO$6</c:f>
+              <c:f>Sheet1!$AO$6:$AO$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -38156,7 +38156,7 @@
           <c:order val="15"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AX$6</c:f>
+              <c:f>Sheet1!$AX$6:$AX$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -39248,7 +39248,7 @@
           <c:order val="16"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AT$6</c:f>
+              <c:f>Sheet1!$AT$6:$AT$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -40355,7 +40355,7 @@
           <c:order val="17"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$BB$6</c:f>
+              <c:f>Sheet1!$BB$6:$BB$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -41450,11 +41450,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="35159912"/>
-        <c:axId val="39037296"/>
+        <c:axId val="38577016"/>
+        <c:axId val="34069276"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="35159912"/>
+        <c:axId val="38577016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -41486,14 +41486,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39037296"/>
+        <c:crossAx val="34069276"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39037296"/>
+        <c:axId val="34069276"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.8"/>
@@ -41537,7 +41537,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35159912"/>
+        <c:crossAx val="38577016"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -41612,9 +41612,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>100</xdr:col>
-      <xdr:colOff>474480</xdr:colOff>
+      <xdr:colOff>474120</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>122040</xdr:rowOff>
+      <xdr:rowOff>121680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -41622,8 +41622,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="40846680" y="0"/>
-        <a:ext cx="22879800" cy="10789920"/>
+        <a:off x="40886640" y="0"/>
+        <a:ext cx="22902480" cy="10789560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -41642,9 +41642,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>83</xdr:col>
-      <xdr:colOff>30240</xdr:colOff>
+      <xdr:colOff>29880</xdr:colOff>
       <xdr:row>155</xdr:row>
-      <xdr:rowOff>92880</xdr:rowOff>
+      <xdr:rowOff>92520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -41652,8 +41652,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="29693520" y="12911400"/>
-        <a:ext cx="22826160" cy="10803240"/>
+        <a:off x="29722320" y="12911400"/>
+        <a:ext cx="22849200" cy="10802880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -41672,9 +41672,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>300240</xdr:colOff>
+      <xdr:colOff>299880</xdr:colOff>
       <xdr:row>182</xdr:row>
-      <xdr:rowOff>138600</xdr:rowOff>
+      <xdr:rowOff>138240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -41685,8 +41685,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15136920" y="27656280"/>
-          <a:ext cx="300240" cy="300240"/>
+          <a:off x="15151680" y="27656280"/>
+          <a:ext cx="299880" cy="299880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -41714,9 +41714,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>617760</xdr:colOff>
+      <xdr:colOff>617400</xdr:colOff>
       <xdr:row>182</xdr:row>
-      <xdr:rowOff>138600</xdr:rowOff>
+      <xdr:rowOff>138240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -41727,8 +41727,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15454440" y="27656280"/>
-          <a:ext cx="300240" cy="300240"/>
+          <a:off x="15469200" y="27656280"/>
+          <a:ext cx="299880" cy="299880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -41756,9 +41756,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>262440</xdr:colOff>
+      <xdr:colOff>262080</xdr:colOff>
       <xdr:row>182</xdr:row>
-      <xdr:rowOff>138600</xdr:rowOff>
+      <xdr:rowOff>138240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -41769,8 +41769,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15782760" y="27656280"/>
-          <a:ext cx="249840" cy="300240"/>
+          <a:off x="15797880" y="27656280"/>
+          <a:ext cx="249480" cy="299880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -41799,11 +41799,11 @@
   </sheetPr>
   <dimension ref="A1:BL284"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AD147" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AR192" activeCellId="0" sqref="AR192"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P160" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="W194" activeCellId="0" sqref="W194"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.16"/>
   </cols>

</xml_diff>

<commit_message>
Spanish graphs on labour-market state scenarios, and updated graphics on adequacy with March 2021, public macroeconomic projections
</commit_message>
<xml_diff>
--- a/Excel_files_for_MISSAR/Prospective_scenarios/2014_q4_start/Historical_graphs_ages_16_69/Economic_scenarios_representation_nov_2020.xlsx
+++ b/Excel_files_for_MISSAR/Prospective_scenarios/2014_q4_start/Historical_graphs_ages_16_69/Economic_scenarios_representation_nov_2020.xlsx
@@ -20,18 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="210">
   <si>
     <t xml:space="preserve">MEN</t>
   </si>
   <si>
     <t xml:space="preserve">WOMEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">period</t>
-  </si>
-  <si>
-    <t xml:space="preserve">period2</t>
   </si>
   <si>
     <t xml:space="preserve">Formal wage-earners</t>
@@ -86,6 +80,51 @@
   </si>
   <si>
     <t xml:space="preserve">Inactive, high scenario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">period</t>
+  </si>
+  <si>
+    <t xml:space="preserve">period2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asalariados formales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trabajadores independientes del sector formal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trabajadores no registrados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desempleados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inactivos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Escenario central</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Escenario pesimista</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Escenario optimista</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asalariadas formales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trabajadoras independientes del sector formal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trabajadoras no registradas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desempleadas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inactivas</t>
   </si>
   <si>
     <t xml:space="preserve">1974_4</t>
@@ -796,7 +835,7 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFCCC1DA"/>
       <rgbColor rgb="FF878787"/>
-      <rgbColor rgb="FF95B3D7"/>
+      <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF9D3E3B"/>
       <rgbColor rgb="FFFDEADA"/>
       <rgbColor rgb="FFD9D9D9"/>
@@ -816,8 +855,8 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFD7E4BD"/>
       <rgbColor rgb="FFC3D69B"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FF95B3D7"/>
+      <rgbColor rgb="FFFF99FF"/>
       <rgbColor rgb="FFB3A2C7"/>
       <rgbColor rgb="FFFCD5B5"/>
       <rgbColor rgb="FF4F81BD"/>
@@ -841,7 +880,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -852,10 +891,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.052481603256615"/>
-          <c:y val="0.02028763055157"/>
-          <c:w val="0.917300767183341"/>
-          <c:h val="0.625446294504321"/>
+          <c:x val="0.0524706324005569"/>
+          <c:y val="0.0202889845496713"/>
+          <c:w val="0.917285823778761"/>
+          <c:h val="0.758367537624721"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -870,7 +909,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Formal wage-earners</c:v>
+                  <c:v>Asalariados formales</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -885,7 +924,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="square"/>
-            <c:size val="5"/>
+            <c:size val="13"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="4f81bd"/>
@@ -893,7 +932,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
-            <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+            <c:numFmt formatCode="0%" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -2058,7 +2097,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Formal wage-earners, low scenario</c:v>
+                  <c:v>Escenario pesimista</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3147,7 +3186,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Formal wage-earners, central scenario</c:v>
+                  <c:v>Escenario central</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4248,7 +4287,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Formal wage-earners, high scenario</c:v>
+                  <c:v>Escenario optimista</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5337,7 +5376,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Independent workers of the formal sector</c:v>
+                  <c:v>Trabajadores independientes del sector formal</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5347,15 +5386,12 @@
               <a:srgbClr val="9d3e3b"/>
             </a:solidFill>
             <a:ln w="47520">
-              <a:solidFill>
-                <a:srgbClr val="9d3e3b"/>
-              </a:solidFill>
-              <a:round/>
+              <a:noFill/>
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="5"/>
+            <c:symbol val="x"/>
+            <c:size val="13"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="9d3e3b"/>
@@ -5363,7 +5399,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
-            <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+            <c:numFmt formatCode="0%" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -6528,7 +6564,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Independent workers of the formal sector, central scenario</c:v>
+                  <c:v>Escenario central</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7629,7 +7665,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Informal sector workers</c:v>
+                  <c:v>Trabajadores no registrados</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7644,7 +7680,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="square"/>
-            <c:size val="5"/>
+            <c:size val="13"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="9bbb59"/>
@@ -7652,7 +7688,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
-            <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+            <c:numFmt formatCode="0%" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -8817,7 +8853,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Informal sector workers, low scenario</c:v>
+                  <c:v>Escenario pesimista</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -9906,7 +9942,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Informal sector workers, central scenario</c:v>
+                  <c:v>Escenario central</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -11007,7 +11043,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Informal sector workers, high scenario</c:v>
+                  <c:v>Escenario optimista</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -12096,30 +12132,30 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Unemployed</c:v>
+                  <c:v>Desempleados</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="99ccff"/>
+              <a:srgbClr val="ff99ff"/>
             </a:solidFill>
             <a:ln w="47520">
               <a:noFill/>
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="5"/>
+            <c:symbol val="triangle"/>
+            <c:size val="13"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="99ccff"/>
+                <a:srgbClr val="ff99ff"/>
               </a:solidFill>
             </c:spPr>
           </c:marker>
           <c:dLbls>
-            <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+            <c:numFmt formatCode="0%" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -13284,7 +13320,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Unemployed, low scenario</c:v>
+                  <c:v>Escenario pesimista</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -14377,7 +14413,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Unemployed, central scenario</c:v>
+                  <c:v>Escenario central</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -15482,7 +15518,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Unemployed, high scenario</c:v>
+                  <c:v>Escenario optimista</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -16571,7 +16607,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Inactive</c:v>
+                  <c:v>Inactivos</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -16586,15 +16622,52 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="9"/>
+            <c:size val="13"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="fdeada"/>
               </a:solidFill>
             </c:spPr>
           </c:marker>
+          <c:dPt>
+            <c:idx val="50"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="13"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="fdeada"/>
+                </a:solidFill>
+              </c:spPr>
+            </c:marker>
+          </c:dPt>
           <c:dLbls>
-            <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+            <c:numFmt formatCode="0%" sourceLinked="1"/>
+            <c:dLbl>
+              <c:idx val="50"/>
+              <c:numFmt formatCode="0%" sourceLinked="1"/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" lang="es-AR" sz="1000" spc="-1" strike="noStrike">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Calibri"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator>; </c:separator>
+            </c:dLbl>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -17771,7 +17844,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Inactive, low scenario</c:v>
+                  <c:v>Escenario pesimista</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -18860,7 +18933,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Inactive, central scenario</c:v>
+                  <c:v>Escenario central</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -19961,7 +20034,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Inactive, high scenario</c:v>
+                  <c:v>Escenario optimista</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -21049,11 +21122,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="14620874"/>
-        <c:axId val="88312981"/>
+        <c:axId val="23215648"/>
+        <c:axId val="20763351"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="14620874"/>
+        <c:axId val="23215648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21085,17 +21158,17 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88312981"/>
+        <c:crossAx val="20763351"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88312981"/>
+        <c:axId val="20763351"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="0.8"/>
+          <c:max val="0.6"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -21135,7 +21208,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14620874"/>
+        <c:crossAx val="23215648"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -21149,18 +21222,16 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0180967358882653"/>
-          <c:y val="0.708526821158031"/>
-          <c:w val="0.969007669495858"/>
-          <c:h val="0.282777481996245"/>
+          <c:x val="0.0180819946504825"/>
+          <c:y val="0.786865552107318"/>
+          <c:w val="0.969013467644805"/>
+          <c:h val="0.204458237394467"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -21199,7 +21270,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -21210,10 +21281,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0465087086144673"/>
-          <c:y val="0.0268279677397854"/>
-          <c:w val="0.940718656833516"/>
-          <c:h val="0.590881823635273"/>
+          <c:x val="0.0465098051510354"/>
+          <c:y val="0.026829756032529"/>
+          <c:w val="0.940698822754848"/>
+          <c:h val="0.721903746167178"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -21228,7 +21299,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Formal wage-earners</c:v>
+                  <c:v>Asalariadas formales</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -21246,7 +21317,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="diamond"/>
-            <c:size val="9"/>
+            <c:size val="13"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="3d679a"/>
@@ -21254,7 +21325,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
-            <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+            <c:numFmt formatCode="0%" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -22419,7 +22490,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Formal wage-earners, low scenario</c:v>
+                  <c:v>Escenario pesimista</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -23511,7 +23582,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Formal wage-earners, central scenario</c:v>
+                  <c:v>Escenario central</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -24615,7 +24686,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Formal wage-earners, high scenario</c:v>
+                  <c:v>Escenario optimista</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -25707,7 +25778,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Independent workers of the formal sector</c:v>
+                  <c:v>Trabajadoras independientes del sector formal</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -25717,15 +25788,12 @@
               <a:srgbClr val="9d3e3b"/>
             </a:solidFill>
             <a:ln w="12600">
-              <a:solidFill>
-                <a:srgbClr val="9d3e3b"/>
-              </a:solidFill>
-              <a:round/>
+              <a:noFill/>
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="9"/>
+            <c:symbol val="x"/>
+            <c:size val="13"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="9d3e3b"/>
@@ -25733,7 +25801,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
-            <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+            <c:numFmt formatCode="0%" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -26898,7 +26966,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Independent workers of the formal sector, central scenario</c:v>
+                  <c:v>Escenario central</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -28002,7 +28070,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Informal sector workers</c:v>
+                  <c:v>Trabajadoras no registradas</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -28016,8 +28084,8 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="triangle"/>
-            <c:size val="9"/>
+            <c:symbol val="square"/>
+            <c:size val="13"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="c3d69b"/>
@@ -28025,7 +28093,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
-            <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+            <c:numFmt formatCode="0%" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -29190,7 +29258,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Informal sector workers, low scenario</c:v>
+                  <c:v>Escenario pesimista</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -30282,7 +30350,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Informal sector workers, central scenario</c:v>
+                  <c:v>Escenario central</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -31386,7 +31454,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Informal sector workers, high scenario</c:v>
+                  <c:v>Escenario optimista</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -32478,30 +32546,30 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Unemployed</c:v>
+                  <c:v>Desempleadas</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="99ccff"/>
+              <a:srgbClr val="ff99ff"/>
             </a:solidFill>
             <a:ln w="12600">
               <a:noFill/>
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="x"/>
-            <c:size val="9"/>
+            <c:symbol val="triangle"/>
+            <c:size val="13"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="99ccff"/>
+                <a:srgbClr val="ff99ff"/>
               </a:solidFill>
             </c:spPr>
           </c:marker>
           <c:dLbls>
-            <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+            <c:numFmt formatCode="0%" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -33666,7 +33734,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Unemployed, low scenario</c:v>
+                  <c:v>Escenario pesimista</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -34758,7 +34826,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Unemployed, central scenario</c:v>
+                  <c:v>Escenario central</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -35862,7 +35930,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Unemployed, high scenario</c:v>
+                  <c:v>Escenario optimista</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -36954,7 +37022,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Inactive</c:v>
+                  <c:v>Inactivas</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -36969,7 +37037,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="9"/>
+            <c:size val="13"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="fdeada"/>
@@ -36977,7 +37045,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
-            <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+            <c:numFmt formatCode="0%" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -38157,7 +38225,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Inactive, low scenario</c:v>
+                  <c:v>Escenario pesimista</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -39249,7 +39317,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Inactive, central scenario</c:v>
+                  <c:v>Escenario central</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -40353,7 +40421,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Inactive, high scenario</c:v>
+                  <c:v>Escenario optimista</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -41444,11 +41512,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="78007631"/>
-        <c:axId val="22887806"/>
+        <c:axId val="14044509"/>
+        <c:axId val="59284396"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="78007631"/>
+        <c:axId val="14044509"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -41480,14 +41548,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22887806"/>
+        <c:crossAx val="59284396"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="22887806"/>
+        <c:axId val="59284396"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.8"/>
@@ -41531,7 +41599,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78007631"/>
+        <c:crossAx val="14044509"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -41545,18 +41613,16 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.00735268078713329"/>
-          <c:y val="0.685606094450959"/>
-          <c:w val="0.977329608713732"/>
-          <c:h val="0.303030286107854"/>
+          <c:x val="0.00735190381389808"/>
+          <c:y val="0.782928942807626"/>
+          <c:w val="0.977332936215572"/>
+          <c:h val="0.205705905879216"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -41600,15 +41666,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>64</xdr:col>
-      <xdr:colOff>385920</xdr:colOff>
+      <xdr:colOff>411840</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>100</xdr:col>
-      <xdr:colOff>473040</xdr:colOff>
+      <xdr:colOff>498600</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>120600</xdr:rowOff>
+      <xdr:rowOff>89640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -41616,8 +41682,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="41046840" y="0"/>
-        <a:ext cx="22992840" cy="10788480"/>
+        <a:off x="41112720" y="0"/>
+        <a:ext cx="23015160" cy="10788120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -41630,15 +41696,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>46</xdr:col>
-      <xdr:colOff>628560</xdr:colOff>
+      <xdr:colOff>628920</xdr:colOff>
       <xdr:row>84</xdr:row>
-      <xdr:rowOff>109800</xdr:rowOff>
+      <xdr:rowOff>110160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>83</xdr:col>
       <xdr:colOff>28800</xdr:colOff>
       <xdr:row>155</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:rowOff>91080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -41646,8 +41712,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="29836440" y="12911400"/>
-        <a:ext cx="22942440" cy="10801800"/>
+        <a:off x="29865240" y="12942000"/>
+        <a:ext cx="22965480" cy="10801440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -41662,11 +41728,11 @@
       <xdr:col>24</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>181</xdr:row>
-      <xdr:rowOff>1080</xdr:rowOff>
+      <xdr:rowOff>1440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>298800</xdr:colOff>
+      <xdr:colOff>298440</xdr:colOff>
       <xdr:row>182</xdr:row>
       <xdr:rowOff>137160</xdr:rowOff>
     </xdr:to>
@@ -41679,8 +41745,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15210000" y="27656280"/>
-          <a:ext cx="298800" cy="298800"/>
+          <a:off x="15224760" y="27687240"/>
+          <a:ext cx="298440" cy="298440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -41704,11 +41770,11 @@
       <xdr:col>24</xdr:col>
       <xdr:colOff>317520</xdr:colOff>
       <xdr:row>181</xdr:row>
-      <xdr:rowOff>1080</xdr:rowOff>
+      <xdr:rowOff>1440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>616320</xdr:colOff>
+      <xdr:colOff>615960</xdr:colOff>
       <xdr:row>182</xdr:row>
       <xdr:rowOff>137160</xdr:rowOff>
     </xdr:to>
@@ -41721,8 +41787,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15527520" y="27656280"/>
-          <a:ext cx="298800" cy="298800"/>
+          <a:off x="15542280" y="27687240"/>
+          <a:ext cx="298440" cy="298440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -41746,11 +41812,11 @@
       <xdr:col>25</xdr:col>
       <xdr:colOff>12600</xdr:colOff>
       <xdr:row>181</xdr:row>
-      <xdr:rowOff>1080</xdr:rowOff>
+      <xdr:rowOff>1440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>261000</xdr:colOff>
+      <xdr:colOff>260640</xdr:colOff>
       <xdr:row>182</xdr:row>
       <xdr:rowOff>137160</xdr:rowOff>
     </xdr:to>
@@ -41763,8 +41829,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15858720" y="27656280"/>
-          <a:ext cx="248400" cy="298800"/>
+          <a:off x="15874200" y="27687240"/>
+          <a:ext cx="248040" cy="298440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -41793,11 +41859,11 @@
   </sheetPr>
   <dimension ref="A1:BL284"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AT234" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BD276" activeCellId="0" sqref="BD276"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AO71" colorId="64" zoomScale="45" zoomScaleNormal="45" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BQ168" activeCellId="0" sqref="BQ168"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.03125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.16"/>
   </cols>
@@ -41812,128 +41878,236 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="O5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="P5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="R5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="S5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="T5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="U5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="V5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="W5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="AK5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AL5" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="AM5" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="AN5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="AP5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="AQ5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="AR5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="AS5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="AT5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="AU5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="AV5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="AW5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AX5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="AY5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="AZ5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="BA5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="BB5" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="N6" s="0" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="O6" s="0" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="P6" s="0" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="Q6" s="0" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="R6" s="0" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="S6" s="0" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="T6" s="0" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="U6" s="0" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="V6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="W6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH6" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="W6" s="0" t="s">
+      <c r="AI6" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="AH6" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI6" s="0" t="s">
-        <v>3</v>
-      </c>
       <c r="AK6" s="0" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="AL6" s="0" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="AM6" s="0" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="AN6" s="0" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="AO6" s="0" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="AP6" s="0" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="AQ6" s="0" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="AR6" s="0" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="AS6" s="0" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="AT6" s="0" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="AU6" s="0" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="AV6" s="0" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="AW6" s="0" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="AX6" s="0" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="AY6" s="0" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="AZ6" s="0" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="BA6" s="0" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="BB6" s="0" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41942,7 +42116,7 @@
         <v>0.2843990218</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>0</v>
@@ -41985,7 +42159,7 @@
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
       <c r="AH7" s="0" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="AI7" s="0" t="n">
         <v>0</v>
@@ -42025,7 +42199,7 @@
     </row>
     <row r="8" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>1</v>
@@ -42058,7 +42232,7 @@
       <c r="AA8" s="1"/>
       <c r="AB8" s="1"/>
       <c r="AH8" s="0" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="AI8" s="0" t="n">
         <v>1</v>
@@ -42088,7 +42262,7 @@
     </row>
     <row r="9" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>2</v>
@@ -42121,7 +42295,7 @@
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
       <c r="AH9" s="0" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="AI9" s="0" t="n">
         <v>2</v>
@@ -42151,7 +42325,7 @@
     </row>
     <row r="10" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>3</v>
@@ -42184,7 +42358,7 @@
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
       <c r="AH10" s="0" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="AI10" s="0" t="n">
         <v>3</v>
@@ -42214,7 +42388,7 @@
     </row>
     <row r="11" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>4</v>
@@ -42247,7 +42421,7 @@
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
       <c r="AH11" s="0" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="AI11" s="0" t="n">
         <v>4</v>
@@ -42277,7 +42451,7 @@
     </row>
     <row r="12" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>5</v>
@@ -42310,7 +42484,7 @@
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
       <c r="AH12" s="0" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="AI12" s="0" t="n">
         <v>5</v>
@@ -42340,7 +42514,7 @@
     </row>
     <row r="13" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>6</v>
@@ -42373,7 +42547,7 @@
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
       <c r="AH13" s="0" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="AI13" s="0" t="n">
         <v>6</v>
@@ -42403,7 +42577,7 @@
     </row>
     <row r="14" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>7</v>
@@ -42436,7 +42610,7 @@
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
       <c r="AH14" s="0" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="AI14" s="0" t="n">
         <v>7</v>
@@ -42466,7 +42640,7 @@
     </row>
     <row r="15" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>8</v>
@@ -42499,7 +42673,7 @@
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
       <c r="AH15" s="0" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="AI15" s="0" t="n">
         <v>8</v>
@@ -42529,7 +42703,7 @@
     </row>
     <row r="16" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>9</v>
@@ -42562,7 +42736,7 @@
       <c r="AA16" s="1"/>
       <c r="AB16" s="1"/>
       <c r="AH16" s="0" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="AI16" s="0" t="n">
         <v>9</v>
@@ -42592,7 +42766,7 @@
     </row>
     <row r="17" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="0" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>10</v>
@@ -42625,7 +42799,7 @@
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
       <c r="AH17" s="0" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="AI17" s="0" t="n">
         <v>10</v>
@@ -42655,7 +42829,7 @@
     </row>
     <row r="18" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="0" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>11</v>
@@ -42688,7 +42862,7 @@
       <c r="AA18" s="1"/>
       <c r="AB18" s="1"/>
       <c r="AH18" s="0" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="AI18" s="0" t="n">
         <v>11</v>
@@ -42718,7 +42892,7 @@
     </row>
     <row r="19" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="0" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>12</v>
@@ -42751,7 +42925,7 @@
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
       <c r="AH19" s="0" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="AI19" s="0" t="n">
         <v>12</v>
@@ -42781,7 +42955,7 @@
     </row>
     <row r="20" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="0" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>13</v>
@@ -42814,7 +42988,7 @@
       <c r="AA20" s="1"/>
       <c r="AB20" s="1"/>
       <c r="AH20" s="0" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="AI20" s="0" t="n">
         <v>13</v>
@@ -42844,7 +43018,7 @@
     </row>
     <row r="21" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="0" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>14</v>
@@ -42877,7 +43051,7 @@
       <c r="AA21" s="1"/>
       <c r="AB21" s="1"/>
       <c r="AH21" s="0" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="AI21" s="0" t="n">
         <v>14</v>
@@ -42907,7 +43081,7 @@
     </row>
     <row r="22" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="0" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>15</v>
@@ -42940,7 +43114,7 @@
       <c r="AA22" s="1"/>
       <c r="AB22" s="1"/>
       <c r="AH22" s="0" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="AI22" s="0" t="n">
         <v>15</v>
@@ -42970,7 +43144,7 @@
     </row>
     <row r="23" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="0" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>16</v>
@@ -43003,7 +43177,7 @@
       <c r="AA23" s="1"/>
       <c r="AB23" s="1"/>
       <c r="AH23" s="0" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="AI23" s="0" t="n">
         <v>16</v>
@@ -43033,7 +43207,7 @@
     </row>
     <row r="24" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="0" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>17</v>
@@ -43066,7 +43240,7 @@
       <c r="AA24" s="1"/>
       <c r="AB24" s="1"/>
       <c r="AH24" s="0" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="AI24" s="0" t="n">
         <v>17</v>
@@ -43096,7 +43270,7 @@
     </row>
     <row r="25" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="0" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>18</v>
@@ -43129,7 +43303,7 @@
       <c r="AA25" s="1"/>
       <c r="AB25" s="1"/>
       <c r="AH25" s="0" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="AI25" s="0" t="n">
         <v>18</v>
@@ -43159,7 +43333,7 @@
     </row>
     <row r="26" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="0" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>19</v>
@@ -43192,7 +43366,7 @@
       <c r="AA26" s="1"/>
       <c r="AB26" s="1"/>
       <c r="AH26" s="0" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="AI26" s="0" t="n">
         <v>19</v>
@@ -43222,7 +43396,7 @@
     </row>
     <row r="27" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="0" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="D27" s="0" t="n">
         <v>20</v>
@@ -43255,7 +43429,7 @@
       <c r="AA27" s="1"/>
       <c r="AB27" s="1"/>
       <c r="AH27" s="0" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="AI27" s="0" t="n">
         <v>20</v>
@@ -43285,7 +43459,7 @@
     </row>
     <row r="28" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="0" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>21</v>
@@ -43318,7 +43492,7 @@
       <c r="AA28" s="1"/>
       <c r="AB28" s="1"/>
       <c r="AH28" s="0" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="AI28" s="0" t="n">
         <v>21</v>
@@ -43348,7 +43522,7 @@
     </row>
     <row r="29" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="0" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>22</v>
@@ -43381,7 +43555,7 @@
       <c r="AA29" s="1"/>
       <c r="AB29" s="1"/>
       <c r="AH29" s="0" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="AI29" s="0" t="n">
         <v>22</v>
@@ -43411,7 +43585,7 @@
     </row>
     <row r="30" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="0" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>23</v>
@@ -43444,7 +43618,7 @@
       <c r="AA30" s="1"/>
       <c r="AB30" s="1"/>
       <c r="AH30" s="0" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="AI30" s="0" t="n">
         <v>23</v>
@@ -43478,7 +43652,7 @@
         <v>0.221750072</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>24</v>
@@ -43521,7 +43695,7 @@
       <c r="AA31" s="1"/>
       <c r="AB31" s="1"/>
       <c r="AH31" s="0" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="AI31" s="0" t="n">
         <v>24</v>
@@ -43561,7 +43735,7 @@
     </row>
     <row r="32" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="0" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="D32" s="0" t="n">
         <v>25</v>
@@ -43594,7 +43768,7 @@
       <c r="AA32" s="1"/>
       <c r="AB32" s="1"/>
       <c r="AH32" s="0" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="AI32" s="0" t="n">
         <v>25</v>
@@ -43624,7 +43798,7 @@
     </row>
     <row r="33" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="0" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>26</v>
@@ -43657,7 +43831,7 @@
       <c r="AA33" s="1"/>
       <c r="AB33" s="1"/>
       <c r="AH33" s="0" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="AI33" s="0" t="n">
         <v>26</v>
@@ -43687,7 +43861,7 @@
     </row>
     <row r="34" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="0" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="D34" s="0" t="n">
         <v>27</v>
@@ -43720,7 +43894,7 @@
       <c r="AA34" s="1"/>
       <c r="AB34" s="1"/>
       <c r="AH34" s="0" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="AI34" s="0" t="n">
         <v>27</v>
@@ -43754,7 +43928,7 @@
         <v>0.2160148082</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="D35" s="0" t="n">
         <v>28</v>
@@ -43797,7 +43971,7 @@
       <c r="AA35" s="1"/>
       <c r="AB35" s="1"/>
       <c r="AH35" s="0" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="AI35" s="0" t="n">
         <v>28</v>
@@ -43837,7 +44011,7 @@
     </row>
     <row r="36" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="0" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="D36" s="0" t="n">
         <v>29</v>
@@ -43870,7 +44044,7 @@
       <c r="AA36" s="1"/>
       <c r="AB36" s="1"/>
       <c r="AH36" s="0" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="AI36" s="0" t="n">
         <v>29</v>
@@ -43900,7 +44074,7 @@
     </row>
     <row r="37" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="0" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="D37" s="0" t="n">
         <v>30</v>
@@ -43933,7 +44107,7 @@
       <c r="AA37" s="1"/>
       <c r="AB37" s="1"/>
       <c r="AH37" s="0" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="AI37" s="0" t="n">
         <v>30</v>
@@ -43963,7 +44137,7 @@
     </row>
     <row r="38" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="0" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="D38" s="0" t="n">
         <v>31</v>
@@ -43996,7 +44170,7 @@
       <c r="AA38" s="1"/>
       <c r="AB38" s="1"/>
       <c r="AH38" s="0" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="AI38" s="0" t="n">
         <v>31</v>
@@ -44030,7 +44204,7 @@
         <v>0.2147149501</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="D39" s="0" t="n">
         <v>32</v>
@@ -44073,7 +44247,7 @@
       <c r="AA39" s="1"/>
       <c r="AB39" s="1"/>
       <c r="AH39" s="0" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="AI39" s="0" t="n">
         <v>32</v>
@@ -44113,7 +44287,7 @@
     </row>
     <row r="40" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="0" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="D40" s="0" t="n">
         <v>33</v>
@@ -44146,7 +44320,7 @@
       <c r="AA40" s="1"/>
       <c r="AB40" s="1"/>
       <c r="AH40" s="0" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="AI40" s="0" t="n">
         <v>33</v>
@@ -44176,7 +44350,7 @@
     </row>
     <row r="41" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="0" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D41" s="0" t="n">
         <v>34</v>
@@ -44209,7 +44383,7 @@
       <c r="AA41" s="1"/>
       <c r="AB41" s="1"/>
       <c r="AH41" s="0" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="AI41" s="0" t="n">
         <v>34</v>
@@ -44239,7 +44413,7 @@
     </row>
     <row r="42" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="0" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="D42" s="0" t="n">
         <v>35</v>
@@ -44272,7 +44446,7 @@
       <c r="AA42" s="1"/>
       <c r="AB42" s="1"/>
       <c r="AH42" s="0" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="AI42" s="0" t="n">
         <v>35</v>
@@ -44302,7 +44476,7 @@
     </row>
     <row r="43" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="0" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="D43" s="0" t="n">
         <v>36</v>
@@ -44335,7 +44509,7 @@
       <c r="AA43" s="1"/>
       <c r="AB43" s="1"/>
       <c r="AH43" s="0" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="AI43" s="0" t="n">
         <v>36</v>
@@ -44365,7 +44539,7 @@
     </row>
     <row r="44" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="0" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="D44" s="0" t="n">
         <v>37</v>
@@ -44398,7 +44572,7 @@
       <c r="AA44" s="1"/>
       <c r="AB44" s="1"/>
       <c r="AH44" s="0" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="AI44" s="0" t="n">
         <v>37</v>
@@ -44428,7 +44602,7 @@
     </row>
     <row r="45" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="0" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="D45" s="0" t="n">
         <v>38</v>
@@ -44461,7 +44635,7 @@
       <c r="AA45" s="1"/>
       <c r="AB45" s="1"/>
       <c r="AH45" s="0" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="AI45" s="0" t="n">
         <v>38</v>
@@ -44491,7 +44665,7 @@
     </row>
     <row r="46" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="0" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="D46" s="0" t="n">
         <v>39</v>
@@ -44524,7 +44698,7 @@
       <c r="AA46" s="1"/>
       <c r="AB46" s="1"/>
       <c r="AH46" s="0" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="AI46" s="0" t="n">
         <v>39</v>
@@ -44554,7 +44728,7 @@
     </row>
     <row r="47" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="0" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="D47" s="0" t="n">
         <v>40</v>
@@ -44587,7 +44761,7 @@
       <c r="AA47" s="1"/>
       <c r="AB47" s="1"/>
       <c r="AH47" s="0" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="AI47" s="0" t="n">
         <v>40</v>
@@ -44617,7 +44791,7 @@
     </row>
     <row r="48" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="0" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="D48" s="0" t="n">
         <v>41</v>
@@ -44650,7 +44824,7 @@
       <c r="AA48" s="1"/>
       <c r="AB48" s="1"/>
       <c r="AH48" s="0" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="AI48" s="0" t="n">
         <v>41</v>
@@ -44680,7 +44854,7 @@
     </row>
     <row r="49" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="0" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="D49" s="0" t="n">
         <v>42</v>
@@ -44713,7 +44887,7 @@
       <c r="AA49" s="1"/>
       <c r="AB49" s="1"/>
       <c r="AH49" s="0" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="AI49" s="0" t="n">
         <v>42</v>
@@ -44743,7 +44917,7 @@
     </row>
     <row r="50" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="0" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="D50" s="0" t="n">
         <v>43</v>
@@ -44776,7 +44950,7 @@
       <c r="AA50" s="1"/>
       <c r="AB50" s="1"/>
       <c r="AH50" s="0" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="AI50" s="0" t="n">
         <v>43</v>
@@ -44810,7 +44984,7 @@
         <v>0.2023154242</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="D51" s="0" t="n">
         <v>44</v>
@@ -44853,7 +45027,7 @@
       <c r="AA51" s="1"/>
       <c r="AB51" s="1"/>
       <c r="AH51" s="0" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="AI51" s="0" t="n">
         <v>44</v>
@@ -44897,7 +45071,7 @@
         <v>0.1930045604</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="D52" s="0" t="n">
         <v>45</v>
@@ -44940,7 +45114,7 @@
       <c r="AA52" s="1"/>
       <c r="AB52" s="1"/>
       <c r="AH52" s="0" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="AI52" s="0" t="n">
         <v>45</v>
@@ -44984,7 +45158,7 @@
         <v>0.1930045604</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="D53" s="0" t="n">
         <v>46</v>
@@ -45027,7 +45201,7 @@
       <c r="AA53" s="1"/>
       <c r="AB53" s="1"/>
       <c r="AH53" s="0" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="AI53" s="0" t="n">
         <v>46</v>
@@ -45067,7 +45241,7 @@
     </row>
     <row r="54" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="0" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="D54" s="0" t="n">
         <v>47</v>
@@ -45100,7 +45274,7 @@
       <c r="AA54" s="1"/>
       <c r="AB54" s="1"/>
       <c r="AH54" s="0" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="AI54" s="0" t="n">
         <v>47</v>
@@ -45134,7 +45308,7 @@
         <v>0.1930045604</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="D55" s="0" t="n">
         <v>48</v>
@@ -45177,7 +45351,7 @@
       <c r="AA55" s="1"/>
       <c r="AB55" s="1"/>
       <c r="AH55" s="0" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="AI55" s="0" t="n">
         <v>48</v>
@@ -45217,7 +45391,7 @@
     </row>
     <row r="56" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C56" s="0" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="D56" s="0" t="n">
         <v>49</v>
@@ -45250,7 +45424,7 @@
       <c r="AA56" s="1"/>
       <c r="AB56" s="1"/>
       <c r="AH56" s="0" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="AI56" s="0" t="n">
         <v>49</v>
@@ -45284,7 +45458,7 @@
         <v>0.1885730096</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="D57" s="0" t="n">
         <v>50</v>
@@ -45327,7 +45501,7 @@
       <c r="AA57" s="1"/>
       <c r="AB57" s="1"/>
       <c r="AH57" s="0" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="AI57" s="0" t="n">
         <v>50</v>
@@ -45368,7 +45542,7 @@
     <row r="58" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="1"/>
       <c r="C58" s="0" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="D58" s="0" t="n">
         <v>51</v>
@@ -45401,7 +45575,7 @@
       <c r="AA58" s="1"/>
       <c r="AB58" s="1"/>
       <c r="AH58" s="0" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="AI58" s="0" t="n">
         <v>51</v>
@@ -45435,7 +45609,7 @@
         <v>0.1926977049</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="D59" s="0" t="n">
         <v>52</v>
@@ -45478,7 +45652,7 @@
       <c r="AA59" s="1"/>
       <c r="AB59" s="1"/>
       <c r="AH59" s="0" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="AI59" s="0" t="n">
         <v>52</v>
@@ -45519,7 +45693,7 @@
     <row r="60" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="1"/>
       <c r="C60" s="0" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="D60" s="0" t="n">
         <v>53</v>
@@ -45552,7 +45726,7 @@
       <c r="AA60" s="1"/>
       <c r="AB60" s="1"/>
       <c r="AH60" s="0" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="AI60" s="0" t="n">
         <v>53</v>
@@ -45586,7 +45760,7 @@
         <v>0.2046257168</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="D61" s="0" t="n">
         <v>54</v>
@@ -45629,7 +45803,7 @@
       <c r="AA61" s="1"/>
       <c r="AB61" s="1"/>
       <c r="AH61" s="0" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="AI61" s="0" t="n">
         <v>54</v>
@@ -45670,7 +45844,7 @@
     <row r="62" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="1"/>
       <c r="C62" s="0" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="D62" s="0" t="n">
         <v>55</v>
@@ -45703,7 +45877,7 @@
       <c r="AA62" s="1"/>
       <c r="AB62" s="1"/>
       <c r="AH62" s="0" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="AI62" s="0" t="n">
         <v>55</v>
@@ -45737,7 +45911,7 @@
         <v>0.2062431092</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="D63" s="0" t="n">
         <v>56</v>
@@ -45780,7 +45954,7 @@
       <c r="AA63" s="1"/>
       <c r="AB63" s="1"/>
       <c r="AH63" s="0" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="AI63" s="0" t="n">
         <v>56</v>
@@ -45821,7 +45995,7 @@
     <row r="64" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="1"/>
       <c r="C64" s="0" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="D64" s="0" t="n">
         <v>57</v>
@@ -45854,7 +46028,7 @@
       <c r="AA64" s="1"/>
       <c r="AB64" s="1"/>
       <c r="AH64" s="0" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="AI64" s="0" t="n">
         <v>57</v>
@@ -45888,7 +46062,7 @@
         <v>0.1953480597</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="D65" s="0" t="n">
         <v>58</v>
@@ -45931,7 +46105,7 @@
       <c r="AA65" s="1"/>
       <c r="AB65" s="1"/>
       <c r="AH65" s="0" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="AI65" s="0" t="n">
         <v>58</v>
@@ -45972,7 +46146,7 @@
     <row r="66" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="1"/>
       <c r="C66" s="0" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="D66" s="0" t="n">
         <v>59</v>
@@ -46005,7 +46179,7 @@
       <c r="AA66" s="1"/>
       <c r="AB66" s="1"/>
       <c r="AH66" s="0" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="AI66" s="0" t="n">
         <v>59</v>
@@ -46039,7 +46213,7 @@
         <v>0.205824674</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="D67" s="0" t="n">
         <v>60</v>
@@ -46082,7 +46256,7 @@
       <c r="AA67" s="1"/>
       <c r="AB67" s="1"/>
       <c r="AH67" s="0" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="AI67" s="0" t="n">
         <v>60</v>
@@ -46123,7 +46297,7 @@
     <row r="68" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="1"/>
       <c r="C68" s="0" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="D68" s="0" t="n">
         <v>61</v>
@@ -46156,7 +46330,7 @@
       <c r="AA68" s="1"/>
       <c r="AB68" s="1"/>
       <c r="AH68" s="0" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="AI68" s="0" t="n">
         <v>61</v>
@@ -46190,7 +46364,7 @@
         <v>0.1953594758</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="D69" s="0" t="n">
         <v>62</v>
@@ -46233,7 +46407,7 @@
       <c r="AA69" s="1"/>
       <c r="AB69" s="1"/>
       <c r="AH69" s="0" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="AI69" s="0" t="n">
         <v>62</v>
@@ -46274,7 +46448,7 @@
     <row r="70" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="1"/>
       <c r="C70" s="0" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="D70" s="0" t="n">
         <v>63</v>
@@ -46307,7 +46481,7 @@
       <c r="AA70" s="1"/>
       <c r="AB70" s="1"/>
       <c r="AH70" s="0" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="AI70" s="0" t="n">
         <v>63</v>
@@ -46341,7 +46515,7 @@
         <v>0.1981950534</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="D71" s="0" t="n">
         <v>64</v>
@@ -46384,7 +46558,7 @@
       <c r="AA71" s="1"/>
       <c r="AB71" s="1"/>
       <c r="AH71" s="0" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="AI71" s="0" t="n">
         <v>64</v>
@@ -46425,7 +46599,7 @@
     <row r="72" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="1"/>
       <c r="C72" s="0" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="D72" s="0" t="n">
         <v>65</v>
@@ -46458,7 +46632,7 @@
       <c r="AA72" s="1"/>
       <c r="AB72" s="1"/>
       <c r="AH72" s="0" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="AI72" s="0" t="n">
         <v>65</v>
@@ -46492,7 +46666,7 @@
         <v>0.1899033235</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="D73" s="0" t="n">
         <v>66</v>
@@ -46535,7 +46709,7 @@
       <c r="AA73" s="1"/>
       <c r="AB73" s="1"/>
       <c r="AH73" s="0" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="AI73" s="0" t="n">
         <v>66</v>
@@ -46576,7 +46750,7 @@
     <row r="74" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="1"/>
       <c r="C74" s="0" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="D74" s="0" t="n">
         <v>67</v>
@@ -46609,7 +46783,7 @@
       <c r="AA74" s="1"/>
       <c r="AB74" s="1"/>
       <c r="AH74" s="0" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="AI74" s="0" t="n">
         <v>67</v>
@@ -46643,7 +46817,7 @@
         <v>0.1892407115</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="D75" s="0" t="n">
         <v>68</v>
@@ -46686,7 +46860,7 @@
       <c r="AA75" s="1"/>
       <c r="AB75" s="1"/>
       <c r="AH75" s="0" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="AI75" s="0" t="n">
         <v>68</v>
@@ -46727,7 +46901,7 @@
     <row r="76" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="1"/>
       <c r="C76" s="0" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="D76" s="0" t="n">
         <v>69</v>
@@ -46760,7 +46934,7 @@
       <c r="AA76" s="1"/>
       <c r="AB76" s="1"/>
       <c r="AH76" s="0" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="AI76" s="0" t="n">
         <v>69</v>
@@ -46794,7 +46968,7 @@
         <v>0.1932947954</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="D77" s="0" t="n">
         <v>70</v>
@@ -46837,7 +47011,7 @@
       <c r="AA77" s="1"/>
       <c r="AB77" s="1"/>
       <c r="AH77" s="0" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="AI77" s="0" t="n">
         <v>70</v>
@@ -46878,7 +47052,7 @@
     <row r="78" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="1"/>
       <c r="C78" s="0" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="D78" s="0" t="n">
         <v>71</v>
@@ -46911,7 +47085,7 @@
       <c r="AA78" s="1"/>
       <c r="AB78" s="1"/>
       <c r="AH78" s="0" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="AI78" s="0" t="n">
         <v>71</v>
@@ -46945,7 +47119,7 @@
         <v>0.1783317932</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="D79" s="0" t="n">
         <v>72</v>
@@ -46988,7 +47162,7 @@
       <c r="AA79" s="1"/>
       <c r="AB79" s="1"/>
       <c r="AH79" s="0" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="AI79" s="0" t="n">
         <v>72</v>
@@ -47029,7 +47203,7 @@
     <row r="80" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="1"/>
       <c r="C80" s="0" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="D80" s="0" t="n">
         <v>73</v>
@@ -47062,7 +47236,7 @@
       <c r="AA80" s="1"/>
       <c r="AB80" s="1"/>
       <c r="AH80" s="0" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="AI80" s="0" t="n">
         <v>73</v>
@@ -47096,7 +47270,7 @@
         <v>0.1735853086</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="D81" s="0" t="n">
         <v>74</v>
@@ -47139,7 +47313,7 @@
       <c r="AA81" s="1"/>
       <c r="AB81" s="1"/>
       <c r="AH81" s="0" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="AI81" s="0" t="n">
         <v>74</v>
@@ -47180,7 +47354,7 @@
     <row r="82" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="1"/>
       <c r="C82" s="0" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="D82" s="0" t="n">
         <v>75</v>
@@ -47213,7 +47387,7 @@
       <c r="AA82" s="1"/>
       <c r="AB82" s="1"/>
       <c r="AH82" s="0" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="AI82" s="0" t="n">
         <v>75</v>
@@ -47247,7 +47421,7 @@
         <v>0.1694606393</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="D83" s="0" t="n">
         <v>76</v>
@@ -47290,7 +47464,7 @@
       <c r="AA83" s="1"/>
       <c r="AB83" s="1"/>
       <c r="AH83" s="0" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="AI83" s="0" t="n">
         <v>76</v>
@@ -47331,7 +47505,7 @@
     <row r="84" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="1"/>
       <c r="C84" s="0" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="D84" s="0" t="n">
         <v>77</v>
@@ -47364,7 +47538,7 @@
       <c r="AA84" s="1"/>
       <c r="AB84" s="1"/>
       <c r="AH84" s="0" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="AI84" s="0" t="n">
         <v>77</v>
@@ -47398,7 +47572,7 @@
         <v>0.1646670672</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="D85" s="0" t="n">
         <v>78</v>
@@ -47441,7 +47615,7 @@
       <c r="AA85" s="1"/>
       <c r="AB85" s="1"/>
       <c r="AH85" s="0" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="AI85" s="0" t="n">
         <v>78</v>
@@ -47482,7 +47656,7 @@
     <row r="86" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="1"/>
       <c r="C86" s="0" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D86" s="0" t="n">
         <v>79</v>
@@ -47515,7 +47689,7 @@
       <c r="AA86" s="1"/>
       <c r="AB86" s="1"/>
       <c r="AH86" s="0" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="AI86" s="0" t="n">
         <v>79</v>
@@ -47549,7 +47723,7 @@
         <v>0.1661993112</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="D87" s="0" t="n">
         <v>80</v>
@@ -47592,7 +47766,7 @@
       <c r="AA87" s="1"/>
       <c r="AB87" s="1"/>
       <c r="AH87" s="0" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="AI87" s="0" t="n">
         <v>80</v>
@@ -47633,7 +47807,7 @@
     <row r="88" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="1"/>
       <c r="C88" s="0" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="D88" s="0" t="n">
         <v>81</v>
@@ -47666,7 +47840,7 @@
       <c r="AA88" s="1"/>
       <c r="AB88" s="1"/>
       <c r="AH88" s="0" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="AI88" s="0" t="n">
         <v>81</v>
@@ -47700,7 +47874,7 @@
         <v>0.1574391095</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="D89" s="0" t="n">
         <v>82</v>
@@ -47743,7 +47917,7 @@
       <c r="AA89" s="1"/>
       <c r="AB89" s="1"/>
       <c r="AH89" s="0" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="AI89" s="0" t="n">
         <v>82</v>
@@ -47784,7 +47958,7 @@
     <row r="90" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="1"/>
       <c r="C90" s="0" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="D90" s="0" t="n">
         <v>83</v>
@@ -47817,7 +47991,7 @@
       <c r="AA90" s="1"/>
       <c r="AB90" s="1"/>
       <c r="AH90" s="0" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="AI90" s="0" t="n">
         <v>83</v>
@@ -47851,7 +48025,7 @@
         <v>0.1447698886</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="D91" s="0" t="n">
         <v>84</v>
@@ -47894,7 +48068,7 @@
       <c r="AA91" s="1"/>
       <c r="AB91" s="1"/>
       <c r="AH91" s="0" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="AI91" s="0" t="n">
         <v>84</v>
@@ -47935,7 +48109,7 @@
     <row r="92" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="1"/>
       <c r="C92" s="0" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="D92" s="0" t="n">
         <v>85</v>
@@ -47968,7 +48142,7 @@
       <c r="AA92" s="1"/>
       <c r="AB92" s="1"/>
       <c r="AH92" s="0" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="AI92" s="0" t="n">
         <v>85</v>
@@ -48002,7 +48176,7 @@
         <v>0.1417102259</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="D93" s="0" t="n">
         <v>86</v>
@@ -48045,7 +48219,7 @@
       <c r="AA93" s="1"/>
       <c r="AB93" s="1"/>
       <c r="AH93" s="0" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="AI93" s="0" t="n">
         <v>86</v>
@@ -48086,7 +48260,7 @@
     <row r="94" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="1"/>
       <c r="C94" s="0" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="D94" s="0" t="n">
         <v>87</v>
@@ -48119,7 +48293,7 @@
       <c r="AA94" s="1"/>
       <c r="AB94" s="1"/>
       <c r="AH94" s="0" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="AI94" s="0" t="n">
         <v>87</v>
@@ -48153,7 +48327,7 @@
         <v>0.1451474275</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="D95" s="0" t="n">
         <v>88</v>
@@ -48196,7 +48370,7 @@
       <c r="AA95" s="1"/>
       <c r="AB95" s="1"/>
       <c r="AH95" s="0" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="AI95" s="0" t="n">
         <v>88</v>
@@ -48237,7 +48411,7 @@
     <row r="96" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="1"/>
       <c r="C96" s="0" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="D96" s="0" t="n">
         <v>89</v>
@@ -48270,7 +48444,7 @@
       <c r="AA96" s="1"/>
       <c r="AB96" s="1"/>
       <c r="AH96" s="0" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="AI96" s="0" t="n">
         <v>89</v>
@@ -48304,7 +48478,7 @@
         <v>0.1376667795</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="D97" s="0" t="n">
         <v>90</v>
@@ -48347,7 +48521,7 @@
       <c r="AA97" s="1"/>
       <c r="AB97" s="1"/>
       <c r="AH97" s="0" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="AI97" s="0" t="n">
         <v>90</v>
@@ -48388,7 +48562,7 @@
     <row r="98" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="1"/>
       <c r="C98" s="0" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="D98" s="0" t="n">
         <v>91</v>
@@ -48421,7 +48595,7 @@
       <c r="AA98" s="1"/>
       <c r="AB98" s="1"/>
       <c r="AH98" s="0" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="AI98" s="0" t="n">
         <v>91</v>
@@ -48455,7 +48629,7 @@
         <v>0.1431920159</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="D99" s="0" t="n">
         <v>92</v>
@@ -48498,7 +48672,7 @@
       <c r="AA99" s="1"/>
       <c r="AB99" s="1"/>
       <c r="AH99" s="0" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="AI99" s="0" t="n">
         <v>92</v>
@@ -48539,7 +48713,7 @@
     <row r="100" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="1"/>
       <c r="C100" s="0" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="D100" s="0" t="n">
         <v>93</v>
@@ -48572,7 +48746,7 @@
       <c r="AA100" s="1"/>
       <c r="AB100" s="1"/>
       <c r="AH100" s="0" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="AI100" s="0" t="n">
         <v>93</v>
@@ -48606,7 +48780,7 @@
         <v>0.1412140829</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="D101" s="0" t="n">
         <v>94</v>
@@ -48649,7 +48823,7 @@
       <c r="AA101" s="1"/>
       <c r="AB101" s="1"/>
       <c r="AH101" s="0" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="AI101" s="0" t="n">
         <v>94</v>
@@ -48690,7 +48864,7 @@
     <row r="102" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="1"/>
       <c r="C102" s="0" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="D102" s="0" t="n">
         <v>95</v>
@@ -48723,7 +48897,7 @@
       <c r="AA102" s="1"/>
       <c r="AB102" s="1"/>
       <c r="AH102" s="0" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="AI102" s="0" t="n">
         <v>95</v>
@@ -48757,7 +48931,7 @@
         <v>0.1407937251</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="D103" s="0" t="n">
         <v>96</v>
@@ -48800,7 +48974,7 @@
       <c r="AA103" s="1"/>
       <c r="AB103" s="1"/>
       <c r="AH103" s="0" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="AI103" s="0" t="n">
         <v>96</v>
@@ -48841,7 +49015,7 @@
     <row r="104" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="1"/>
       <c r="C104" s="0" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="D104" s="0" t="n">
         <v>97</v>
@@ -48874,7 +49048,7 @@
       <c r="AA104" s="1"/>
       <c r="AB104" s="1"/>
       <c r="AH104" s="0" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="AI104" s="0" t="n">
         <v>97</v>
@@ -48908,7 +49082,7 @@
         <v>0.1262047252</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="D105" s="0" t="n">
         <v>98</v>
@@ -48951,7 +49125,7 @@
       <c r="AA105" s="1"/>
       <c r="AB105" s="1"/>
       <c r="AH105" s="0" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="AI105" s="0" t="n">
         <v>98</v>
@@ -48992,7 +49166,7 @@
     <row r="106" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="1"/>
       <c r="C106" s="0" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="D106" s="0" t="n">
         <v>99</v>
@@ -49025,7 +49199,7 @@
       <c r="AA106" s="1"/>
       <c r="AB106" s="1"/>
       <c r="AH106" s="0" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="AI106" s="0" t="n">
         <v>99</v>
@@ -49059,7 +49233,7 @@
         <v>0.1285626353</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="D107" s="0" t="n">
         <v>100</v>
@@ -49102,7 +49276,7 @@
       <c r="AA107" s="1"/>
       <c r="AB107" s="1"/>
       <c r="AH107" s="0" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="AI107" s="0" t="n">
         <v>100</v>
@@ -49143,7 +49317,7 @@
     <row r="108" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="1"/>
       <c r="C108" s="0" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="D108" s="0" t="n">
         <v>101</v>
@@ -49176,7 +49350,7 @@
       <c r="AA108" s="1"/>
       <c r="AB108" s="1"/>
       <c r="AH108" s="0" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="AI108" s="0" t="n">
         <v>101</v>
@@ -49210,7 +49384,7 @@
         <v>0.124128982</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="D109" s="0" t="n">
         <v>102</v>
@@ -49253,7 +49427,7 @@
       <c r="AA109" s="1"/>
       <c r="AB109" s="1"/>
       <c r="AH109" s="0" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="AI109" s="0" t="n">
         <v>102</v>
@@ -49294,7 +49468,7 @@
     <row r="110" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="1"/>
       <c r="C110" s="0" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="D110" s="0" t="n">
         <v>103</v>
@@ -49327,7 +49501,7 @@
       <c r="AA110" s="1"/>
       <c r="AB110" s="1"/>
       <c r="AH110" s="0" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="AI110" s="0" t="n">
         <v>103</v>
@@ -49361,7 +49535,7 @@
         <v>0.1257338189</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
       <c r="D111" s="0" t="n">
         <v>104</v>
@@ -49404,7 +49578,7 @@
       <c r="AA111" s="1"/>
       <c r="AB111" s="1"/>
       <c r="AH111" s="0" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
       <c r="AI111" s="0" t="n">
         <v>104</v>
@@ -49445,7 +49619,7 @@
     <row r="112" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="1"/>
       <c r="C112" s="0" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="D112" s="0" t="n">
         <v>105</v>
@@ -49478,7 +49652,7 @@
       <c r="AA112" s="1"/>
       <c r="AB112" s="1"/>
       <c r="AH112" s="0" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="AI112" s="0" t="n">
         <v>105</v>
@@ -49512,7 +49686,7 @@
         <v>0.1216132758</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
       <c r="D113" s="0" t="n">
         <v>106</v>
@@ -49555,7 +49729,7 @@
       <c r="AA113" s="1"/>
       <c r="AB113" s="1"/>
       <c r="AH113" s="0" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
       <c r="AI113" s="0" t="n">
         <v>106</v>
@@ -49596,7 +49770,7 @@
     <row r="114" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="1"/>
       <c r="C114" s="0" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="D114" s="0" t="n">
         <v>107</v>
@@ -49629,7 +49803,7 @@
       <c r="AA114" s="1"/>
       <c r="AB114" s="1"/>
       <c r="AH114" s="0" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="AI114" s="0" t="n">
         <v>107</v>
@@ -49663,7 +49837,7 @@
         <v>0.1074732992</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="D115" s="0" t="n">
         <v>108</v>
@@ -49706,7 +49880,7 @@
       <c r="AA115" s="1"/>
       <c r="AB115" s="1"/>
       <c r="AH115" s="0" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="AI115" s="0" t="n">
         <v>108</v>
@@ -49747,7 +49921,7 @@
     <row r="116" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="1"/>
       <c r="C116" s="0" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="D116" s="0" t="n">
         <v>109</v>
@@ -49780,7 +49954,7 @@
       <c r="AA116" s="1"/>
       <c r="AB116" s="1"/>
       <c r="AH116" s="0" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="AI116" s="0" t="n">
         <v>109</v>
@@ -49814,7 +49988,7 @@
         <v>0.0899775179</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="D117" s="0" t="n">
         <v>110</v>
@@ -49857,7 +50031,7 @@
       <c r="AA117" s="1"/>
       <c r="AB117" s="1"/>
       <c r="AH117" s="0" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="AI117" s="0" t="n">
         <v>110</v>
@@ -49898,7 +50072,7 @@
     <row r="118" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="1"/>
       <c r="C118" s="0" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="D118" s="0" t="n">
         <v>111</v>
@@ -49931,7 +50105,7 @@
       <c r="AA118" s="1"/>
       <c r="AB118" s="1"/>
       <c r="AH118" s="0" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="AI118" s="0" t="n">
         <v>111</v>
@@ -49965,7 +50139,7 @@
         <v>0.0801653696</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="D119" s="0" t="n">
         <v>112</v>
@@ -50008,7 +50182,7 @@
       <c r="AA119" s="1"/>
       <c r="AB119" s="1"/>
       <c r="AH119" s="0" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="AI119" s="0" t="n">
         <v>112</v>
@@ -50049,7 +50223,7 @@
     <row r="120" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="1"/>
       <c r="C120" s="0" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="D120" s="0" t="n">
         <v>113</v>
@@ -50082,7 +50256,7 @@
       <c r="AA120" s="1"/>
       <c r="AB120" s="1"/>
       <c r="AH120" s="0" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="AI120" s="0" t="n">
         <v>113</v>
@@ -50116,7 +50290,7 @@
         <v>0.0788367316</v>
       </c>
       <c r="C121" s="0" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="D121" s="0" t="n">
         <v>114</v>
@@ -50159,7 +50333,7 @@
       <c r="AA121" s="1"/>
       <c r="AB121" s="1"/>
       <c r="AH121" s="0" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="AI121" s="0" t="n">
         <v>114</v>
@@ -50203,7 +50377,7 @@
         <v>0.0985742349</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="D122" s="0" t="n">
         <v>115</v>
@@ -50246,7 +50420,7 @@
       <c r="AA122" s="1"/>
       <c r="AB122" s="1"/>
       <c r="AH122" s="0" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="AI122" s="0" t="n">
         <v>115</v>
@@ -50290,7 +50464,7 @@
         <v>0.1192286447</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="D123" s="0" t="n">
         <v>116</v>
@@ -50333,7 +50507,7 @@
       <c r="AA123" s="1"/>
       <c r="AB123" s="1"/>
       <c r="AH123" s="0" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="AI123" s="0" t="n">
         <v>116</v>
@@ -50377,7 +50551,7 @@
         <v>0.1202145345</v>
       </c>
       <c r="C124" s="0" t="s">
-        <v>139</v>
+        <v>152</v>
       </c>
       <c r="D124" s="0" t="n">
         <v>117</v>
@@ -50420,7 +50594,7 @@
       <c r="AA124" s="1"/>
       <c r="AB124" s="1"/>
       <c r="AH124" s="0" t="s">
-        <v>139</v>
+        <v>152</v>
       </c>
       <c r="AI124" s="0" t="n">
         <v>117</v>
@@ -50464,7 +50638,7 @@
         <v>0.1205344478</v>
       </c>
       <c r="C125" s="0" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
       <c r="D125" s="0" t="n">
         <v>118</v>
@@ -50507,7 +50681,7 @@
       <c r="AA125" s="1"/>
       <c r="AB125" s="1"/>
       <c r="AH125" s="0" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
       <c r="AI125" s="0" t="n">
         <v>118</v>
@@ -50551,7 +50725,7 @@
         <v>0.1194938208</v>
       </c>
       <c r="C126" s="0" t="s">
-        <v>141</v>
+        <v>154</v>
       </c>
       <c r="D126" s="0" t="n">
         <v>119</v>
@@ -50594,7 +50768,7 @@
       <c r="AA126" s="1"/>
       <c r="AB126" s="1"/>
       <c r="AH126" s="0" t="s">
-        <v>141</v>
+        <v>154</v>
       </c>
       <c r="AI126" s="0" t="n">
         <v>119</v>
@@ -50638,7 +50812,7 @@
         <v>0.1303682252</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="D127" s="0" t="n">
         <v>120</v>
@@ -50681,7 +50855,7 @@
       <c r="AA127" s="1"/>
       <c r="AB127" s="1"/>
       <c r="AH127" s="0" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="AI127" s="0" t="n">
         <v>120</v>
@@ -50725,7 +50899,7 @@
         <v>0.1348205942</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="D128" s="0" t="n">
         <v>121</v>
@@ -50768,7 +50942,7 @@
       <c r="AA128" s="1"/>
       <c r="AB128" s="1"/>
       <c r="AH128" s="0" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="AI128" s="0" t="n">
         <v>121</v>
@@ -50812,7 +50986,7 @@
         <v>0.1373907125</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="D129" s="0" t="n">
         <v>122</v>
@@ -50855,7 +51029,7 @@
       <c r="AA129" s="1"/>
       <c r="AB129" s="1"/>
       <c r="AH129" s="0" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="AI129" s="0" t="n">
         <v>122</v>
@@ -50899,7 +51073,7 @@
         <v>0.1279769945</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="D130" s="0" t="n">
         <v>123</v>
@@ -50942,7 +51116,7 @@
       <c r="AA130" s="1"/>
       <c r="AB130" s="1"/>
       <c r="AH130" s="0" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="AI130" s="0" t="n">
         <v>123</v>
@@ -50986,7 +51160,7 @@
         <v>0.1219682845</v>
       </c>
       <c r="C131" s="0" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="D131" s="0" t="n">
         <v>124</v>
@@ -51029,7 +51203,7 @@
       <c r="AA131" s="1"/>
       <c r="AB131" s="1"/>
       <c r="AH131" s="0" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="AI131" s="0" t="n">
         <v>124</v>
@@ -51073,7 +51247,7 @@
         <v>0.1430198679</v>
       </c>
       <c r="C132" s="0" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
       <c r="D132" s="0" t="n">
         <v>125</v>
@@ -51116,7 +51290,7 @@
       <c r="AA132" s="1"/>
       <c r="AB132" s="1"/>
       <c r="AH132" s="0" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
       <c r="AI132" s="0" t="n">
         <v>125</v>
@@ -51160,7 +51334,7 @@
         <v>0.1343898815</v>
       </c>
       <c r="C133" s="0" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="D133" s="0" t="n">
         <v>126</v>
@@ -51203,7 +51377,7 @@
       <c r="AA133" s="1"/>
       <c r="AB133" s="1"/>
       <c r="AH133" s="0" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="AI133" s="0" t="n">
         <v>126</v>
@@ -51247,7 +51421,7 @@
         <v>0.137221854</v>
       </c>
       <c r="C134" s="0" t="s">
-        <v>149</v>
+        <v>162</v>
       </c>
       <c r="D134" s="0" t="n">
         <v>127</v>
@@ -51290,7 +51464,7 @@
       <c r="AA134" s="1"/>
       <c r="AB134" s="1"/>
       <c r="AH134" s="0" t="s">
-        <v>149</v>
+        <v>162</v>
       </c>
       <c r="AI134" s="0" t="n">
         <v>127</v>
@@ -51334,7 +51508,7 @@
         <v>0.1360900758</v>
       </c>
       <c r="C135" s="0" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="D135" s="0" t="n">
         <v>128</v>
@@ -51377,7 +51551,7 @@
       <c r="AA135" s="1"/>
       <c r="AB135" s="1"/>
       <c r="AH135" s="0" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="AI135" s="0" t="n">
         <v>128</v>
@@ -51421,7 +51595,7 @@
         <v>0.1497488399</v>
       </c>
       <c r="C136" s="0" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="D136" s="0" t="n">
         <v>129</v>
@@ -51464,7 +51638,7 @@
       <c r="AA136" s="1"/>
       <c r="AB136" s="1"/>
       <c r="AH136" s="0" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="AI136" s="0" t="n">
         <v>129</v>
@@ -51508,7 +51682,7 @@
         <v>0.1468165257</v>
       </c>
       <c r="C137" s="0" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
       <c r="D137" s="0" t="n">
         <v>130</v>
@@ -51551,7 +51725,7 @@
       <c r="AA137" s="1"/>
       <c r="AB137" s="1"/>
       <c r="AH137" s="0" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
       <c r="AI137" s="0" t="n">
         <v>130</v>
@@ -51592,7 +51766,7 @@
     <row r="138" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B138" s="1"/>
       <c r="C138" s="0" t="s">
-        <v>153</v>
+        <v>166</v>
       </c>
       <c r="D138" s="0" t="n">
         <v>131</v>
@@ -51625,7 +51799,7 @@
       <c r="AA138" s="1"/>
       <c r="AB138" s="1"/>
       <c r="AH138" s="0" t="s">
-        <v>153</v>
+        <v>166</v>
       </c>
       <c r="AI138" s="0" t="n">
         <v>131</v>
@@ -51659,7 +51833,7 @@
         <v>0.1567389734</v>
       </c>
       <c r="C139" s="0" t="s">
-        <v>154</v>
+        <v>167</v>
       </c>
       <c r="D139" s="0" t="n">
         <v>132</v>
@@ -51702,7 +51876,7 @@
       <c r="AA139" s="1"/>
       <c r="AB139" s="1"/>
       <c r="AH139" s="0" t="s">
-        <v>154</v>
+        <v>167</v>
       </c>
       <c r="AI139" s="0" t="n">
         <v>132</v>
@@ -51746,7 +51920,7 @@
         <v>0.1396718689</v>
       </c>
       <c r="C140" s="0" t="s">
-        <v>155</v>
+        <v>168</v>
       </c>
       <c r="D140" s="0" t="n">
         <v>133</v>
@@ -51789,7 +51963,7 @@
       <c r="AA140" s="1"/>
       <c r="AB140" s="1"/>
       <c r="AH140" s="0" t="s">
-        <v>155</v>
+        <v>168</v>
       </c>
       <c r="AI140" s="0" t="n">
         <v>133</v>
@@ -51833,7 +52007,7 @@
         <v>0.1464966508</v>
       </c>
       <c r="C141" s="0" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="D141" s="0" t="n">
         <v>134</v>
@@ -51876,7 +52050,7 @@
       <c r="AA141" s="1"/>
       <c r="AB141" s="1"/>
       <c r="AH141" s="0" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="AI141" s="0" t="n">
         <v>134</v>
@@ -51920,7 +52094,7 @@
         <v>0.1511412362</v>
       </c>
       <c r="C142" s="0" t="s">
-        <v>157</v>
+        <v>170</v>
       </c>
       <c r="D142" s="0" t="n">
         <v>135</v>
@@ -51963,7 +52137,7 @@
       <c r="AA142" s="1"/>
       <c r="AB142" s="1"/>
       <c r="AH142" s="0" t="s">
-        <v>157</v>
+        <v>170</v>
       </c>
       <c r="AI142" s="0" t="n">
         <v>135</v>
@@ -52007,7 +52181,7 @@
         <v>0.142844428</v>
       </c>
       <c r="C143" s="0" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="D143" s="0" t="n">
         <v>136</v>
@@ -52050,7 +52224,7 @@
       <c r="AA143" s="1"/>
       <c r="AB143" s="1"/>
       <c r="AH143" s="0" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="AI143" s="0" t="n">
         <v>136</v>
@@ -52094,7 +52268,7 @@
         <v>0.1355907701</v>
       </c>
       <c r="C144" s="0" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="D144" s="0" t="n">
         <v>137</v>
@@ -52137,7 +52311,7 @@
       <c r="AA144" s="1"/>
       <c r="AB144" s="1"/>
       <c r="AH144" s="0" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="AI144" s="0" t="n">
         <v>137</v>
@@ -52181,7 +52355,7 @@
         <v>0.1323540236</v>
       </c>
       <c r="C145" s="0" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
       <c r="D145" s="0" t="n">
         <v>138</v>
@@ -52224,7 +52398,7 @@
       <c r="AA145" s="1"/>
       <c r="AB145" s="1"/>
       <c r="AH145" s="0" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
       <c r="AI145" s="0" t="n">
         <v>138</v>
@@ -52268,7 +52442,7 @@
         <v>0.1285650329</v>
       </c>
       <c r="C146" s="0" t="s">
-        <v>161</v>
+        <v>174</v>
       </c>
       <c r="D146" s="0" t="n">
         <v>139</v>
@@ -52311,7 +52485,7 @@
       <c r="AA146" s="1"/>
       <c r="AB146" s="1"/>
       <c r="AH146" s="0" t="s">
-        <v>161</v>
+        <v>174</v>
       </c>
       <c r="AI146" s="0" t="n">
         <v>139</v>
@@ -52355,7 +52529,7 @@
         <v>0.1145466074</v>
       </c>
       <c r="C147" s="0" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="D147" s="0" t="n">
         <v>140</v>
@@ -52398,7 +52572,7 @@
       <c r="AA147" s="1"/>
       <c r="AB147" s="1"/>
       <c r="AH147" s="0" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="AI147" s="0" t="n">
         <v>140</v>
@@ -52442,7 +52616,7 @@
         <v>0.1316293675</v>
       </c>
       <c r="C148" s="0" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="D148" s="0" t="n">
         <v>141</v>
@@ -52485,7 +52659,7 @@
       <c r="AA148" s="1"/>
       <c r="AB148" s="1"/>
       <c r="AH148" s="0" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="AI148" s="0" t="n">
         <v>141</v>
@@ -52529,7 +52703,7 @@
         <v>0.1389852344</v>
       </c>
       <c r="C149" s="0" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="D149" s="0" t="n">
         <v>142</v>
@@ -52572,7 +52746,7 @@
       <c r="AA149" s="1"/>
       <c r="AB149" s="1"/>
       <c r="AH149" s="0" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="AI149" s="0" t="n">
         <v>142</v>
@@ -52616,7 +52790,7 @@
         <v>0.1433559766</v>
       </c>
       <c r="C150" s="0" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="D150" s="0" t="n">
         <v>143</v>
@@ -52659,7 +52833,7 @@
       <c r="AA150" s="1"/>
       <c r="AB150" s="1"/>
       <c r="AH150" s="0" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="AI150" s="0" t="n">
         <v>143</v>
@@ -52703,7 +52877,7 @@
         <v>0.1378898272</v>
       </c>
       <c r="C151" s="0" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
       <c r="D151" s="0" t="n">
         <v>144</v>
@@ -52746,7 +52920,7 @@
       <c r="AA151" s="1"/>
       <c r="AB151" s="1"/>
       <c r="AH151" s="0" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
       <c r="AI151" s="0" t="n">
         <v>144</v>
@@ -52790,7 +52964,7 @@
         <v>0.1340250847</v>
       </c>
       <c r="C152" s="0" t="s">
-        <v>167</v>
+        <v>180</v>
       </c>
       <c r="D152" s="0" t="n">
         <v>145</v>
@@ -52833,7 +53007,7 @@
       <c r="AA152" s="1"/>
       <c r="AB152" s="1"/>
       <c r="AH152" s="0" t="s">
-        <v>167</v>
+        <v>180</v>
       </c>
       <c r="AI152" s="0" t="n">
         <v>145</v>
@@ -52877,7 +53051,7 @@
         <v>0.1396290821</v>
       </c>
       <c r="C153" s="0" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="D153" s="0" t="n">
         <v>146</v>
@@ -52920,7 +53094,7 @@
       <c r="AA153" s="1"/>
       <c r="AB153" s="1"/>
       <c r="AH153" s="0" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="AI153" s="0" t="n">
         <v>146</v>
@@ -52964,7 +53138,7 @@
         <v>0.1454228549</v>
       </c>
       <c r="C154" s="0" t="s">
-        <v>169</v>
+        <v>182</v>
       </c>
       <c r="D154" s="0" t="n">
         <v>147</v>
@@ -53007,7 +53181,7 @@
       <c r="AA154" s="1"/>
       <c r="AB154" s="1"/>
       <c r="AH154" s="0" t="s">
-        <v>169</v>
+        <v>182</v>
       </c>
       <c r="AI154" s="0" t="n">
         <v>147</v>
@@ -53051,7 +53225,7 @@
         <v>0.141814718</v>
       </c>
       <c r="C155" s="0" t="s">
-        <v>170</v>
+        <v>183</v>
       </c>
       <c r="D155" s="0" t="n">
         <v>148</v>
@@ -53094,7 +53268,7 @@
       <c r="AA155" s="1"/>
       <c r="AB155" s="1"/>
       <c r="AH155" s="0" t="s">
-        <v>170</v>
+        <v>183</v>
       </c>
       <c r="AI155" s="0" t="n">
         <v>148</v>
@@ -53138,7 +53312,7 @@
         <v>0.1329188961</v>
       </c>
       <c r="C156" s="0" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
       <c r="D156" s="0" t="n">
         <v>149</v>
@@ -53181,7 +53355,7 @@
       <c r="AA156" s="1"/>
       <c r="AB156" s="1"/>
       <c r="AH156" s="0" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
       <c r="AI156" s="0" t="n">
         <v>149</v>
@@ -53225,7 +53399,7 @@
         <v>0.1236320225</v>
       </c>
       <c r="C157" s="0" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="D157" s="0" t="n">
         <v>150</v>
@@ -53268,7 +53442,7 @@
       <c r="AA157" s="1"/>
       <c r="AB157" s="1"/>
       <c r="AH157" s="0" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="AI157" s="0" t="n">
         <v>150</v>
@@ -53312,7 +53486,7 @@
         <v>0.1362855228</v>
       </c>
       <c r="C158" s="0" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="D158" s="0" t="n">
         <v>151</v>
@@ -53355,7 +53529,7 @@
       <c r="AA158" s="1"/>
       <c r="AB158" s="1"/>
       <c r="AH158" s="0" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="AI158" s="0" t="n">
         <v>151</v>
@@ -53399,7 +53573,7 @@
         <v>0.139175282</v>
       </c>
       <c r="C159" s="0" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="D159" s="0" t="n">
         <v>152</v>
@@ -53442,7 +53616,7 @@
       <c r="AA159" s="1"/>
       <c r="AB159" s="1"/>
       <c r="AH159" s="0" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="AI159" s="0" t="n">
         <v>152</v>
@@ -53486,7 +53660,7 @@
         <v>0.1366378981</v>
       </c>
       <c r="C160" s="0" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
       <c r="D160" s="0" t="n">
         <v>153</v>
@@ -53529,7 +53703,7 @@
       <c r="AA160" s="1"/>
       <c r="AB160" s="1"/>
       <c r="AH160" s="0" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
       <c r="AI160" s="0" t="n">
         <v>153</v>
@@ -53573,7 +53747,7 @@
         <v>0.1179233816</v>
       </c>
       <c r="C161" s="0" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="D161" s="0" t="n">
         <v>154</v>
@@ -53616,7 +53790,7 @@
       <c r="AA161" s="1"/>
       <c r="AB161" s="1"/>
       <c r="AH161" s="0" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="AI161" s="0" t="n">
         <v>154</v>
@@ -53660,7 +53834,7 @@
         <v>0.113989806</v>
       </c>
       <c r="C162" s="0" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="D162" s="0" t="n">
         <v>155</v>
@@ -53703,7 +53877,7 @@
       <c r="AA162" s="1"/>
       <c r="AB162" s="1"/>
       <c r="AH162" s="0" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="AI162" s="0" t="n">
         <v>155</v>
@@ -53747,7 +53921,7 @@
         <v>0.1111436188</v>
       </c>
       <c r="C163" s="0" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="D163" s="0" t="n">
         <v>156</v>
@@ -53790,7 +53964,7 @@
       <c r="AA163" s="1"/>
       <c r="AB163" s="1"/>
       <c r="AH163" s="0" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="AI163" s="0" t="n">
         <v>156</v>
@@ -53834,7 +54008,7 @@
         <v>0.1292437922</v>
       </c>
       <c r="C164" s="0" t="s">
-        <v>179</v>
+        <v>192</v>
       </c>
       <c r="D164" s="0" t="n">
         <v>157</v>
@@ -53877,7 +54051,7 @@
       <c r="AA164" s="1"/>
       <c r="AB164" s="1"/>
       <c r="AH164" s="0" t="s">
-        <v>179</v>
+        <v>192</v>
       </c>
       <c r="AI164" s="0" t="n">
         <v>157</v>
@@ -53921,7 +54095,7 @@
         <v>0.1310061393</v>
       </c>
       <c r="C165" s="0" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
       <c r="D165" s="0" t="n">
         <v>158</v>
@@ -53964,7 +54138,7 @@
       <c r="AA165" s="1"/>
       <c r="AB165" s="1"/>
       <c r="AH165" s="0" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
       <c r="AI165" s="0" t="n">
         <v>158</v>
@@ -54008,7 +54182,7 @@
         <v>0.1194103348</v>
       </c>
       <c r="C166" s="0" t="s">
-        <v>181</v>
+        <v>194</v>
       </c>
       <c r="D166" s="0" t="n">
         <v>159</v>
@@ -54051,7 +54225,7 @@
       <c r="AA166" s="1"/>
       <c r="AB166" s="1"/>
       <c r="AH166" s="0" t="s">
-        <v>181</v>
+        <v>194</v>
       </c>
       <c r="AI166" s="0" t="n">
         <v>159</v>
@@ -54095,7 +54269,7 @@
         <v>0.1103959014</v>
       </c>
       <c r="C167" s="0" t="s">
-        <v>182</v>
+        <v>195</v>
       </c>
       <c r="D167" s="0" t="n">
         <v>160</v>
@@ -54138,7 +54312,7 @@
       <c r="AA167" s="1"/>
       <c r="AB167" s="1"/>
       <c r="AH167" s="0" t="s">
-        <v>182</v>
+        <v>195</v>
       </c>
       <c r="AI167" s="0" t="n">
         <v>160</v>
@@ -54182,7 +54356,7 @@
         <v>0.1169026145</v>
       </c>
       <c r="C168" s="0" t="s">
-        <v>183</v>
+        <v>196</v>
       </c>
       <c r="D168" s="0" t="n">
         <v>161</v>
@@ -54225,7 +54399,7 @@
       <c r="AA168" s="1"/>
       <c r="AB168" s="1"/>
       <c r="AH168" s="0" t="s">
-        <v>183</v>
+        <v>196</v>
       </c>
       <c r="AI168" s="0" t="n">
         <v>161</v>
@@ -54269,7 +54443,7 @@
         <v>0.1232194249</v>
       </c>
       <c r="C169" s="0" t="s">
-        <v>184</v>
+        <v>197</v>
       </c>
       <c r="D169" s="0" t="n">
         <v>162</v>
@@ -54312,7 +54486,7 @@
       <c r="AA169" s="1"/>
       <c r="AB169" s="1"/>
       <c r="AH169" s="0" t="s">
-        <v>184</v>
+        <v>197</v>
       </c>
       <c r="AI169" s="0" t="n">
         <v>162</v>
@@ -54353,7 +54527,7 @@
     <row r="170" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B170" s="1"/>
       <c r="C170" s="0" t="s">
-        <v>185</v>
+        <v>198</v>
       </c>
       <c r="D170" s="0" t="n">
         <v>163</v>
@@ -54386,7 +54560,7 @@
       <c r="AA170" s="1"/>
       <c r="AB170" s="1"/>
       <c r="AH170" s="0" t="s">
-        <v>185</v>
+        <v>198</v>
       </c>
       <c r="AI170" s="0" t="n">
         <v>163</v>
@@ -54417,7 +54591,7 @@
     <row r="171" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B171" s="1"/>
       <c r="C171" s="0" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="D171" s="0" t="n">
         <v>164</v>
@@ -54450,7 +54624,7 @@
       <c r="AA171" s="1"/>
       <c r="AB171" s="1"/>
       <c r="AH171" s="0" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="AI171" s="0" t="n">
         <v>164</v>
@@ -54481,7 +54655,7 @@
     <row r="172" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B172" s="1"/>
       <c r="C172" s="0" t="s">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="D172" s="0" t="n">
         <v>165</v>
@@ -54514,7 +54688,7 @@
       <c r="AA172" s="1"/>
       <c r="AB172" s="1"/>
       <c r="AH172" s="0" t="s">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="AI172" s="0" t="n">
         <v>165</v>
@@ -54548,7 +54722,7 @@
         <v>0.1051070485</v>
       </c>
       <c r="C173" s="0" t="s">
-        <v>188</v>
+        <v>201</v>
       </c>
       <c r="D173" s="0" t="n">
         <v>166</v>
@@ -54590,7 +54764,7 @@
       <c r="AA173" s="1"/>
       <c r="AB173" s="1"/>
       <c r="AH173" s="0" t="s">
-        <v>188</v>
+        <v>201</v>
       </c>
       <c r="AI173" s="0" t="n">
         <v>166</v>
@@ -54633,7 +54807,7 @@
         <v>0.1096864667</v>
       </c>
       <c r="C174" s="0" t="s">
-        <v>189</v>
+        <v>202</v>
       </c>
       <c r="D174" s="0" t="n">
         <v>167</v>
@@ -54675,7 +54849,7 @@
       <c r="AA174" s="1"/>
       <c r="AB174" s="1"/>
       <c r="AH174" s="0" t="s">
-        <v>189</v>
+        <v>202</v>
       </c>
       <c r="AI174" s="0" t="n">
         <v>167</v>
@@ -54718,7 +54892,7 @@
         <v>0.103301065</v>
       </c>
       <c r="C175" s="0" t="s">
-        <v>190</v>
+        <v>203</v>
       </c>
       <c r="D175" s="0" t="n">
         <v>168</v>
@@ -54777,7 +54951,7 @@
         <v>0.01276852714</v>
       </c>
       <c r="AH175" s="0" t="s">
-        <v>190</v>
+        <v>203</v>
       </c>
       <c r="AI175" s="0" t="n">
         <v>168</v>
@@ -54846,7 +55020,7 @@
         <v>0.1021125894</v>
       </c>
       <c r="C176" s="0" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
       <c r="D176" s="0" t="n">
         <v>169</v>
@@ -54883,7 +55057,7 @@
       <c r="X176" s="1"/>
       <c r="Y176" s="1"/>
       <c r="AH176" s="0" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
       <c r="AI176" s="0" t="n">
         <v>169</v>
@@ -56799,7 +56973,7 @@
         <v>0.417307752531169</v>
       </c>
       <c r="BC195" s="5" t="s">
-        <v>192</v>
+        <v>205</v>
       </c>
       <c r="BD195" s="5"/>
       <c r="BE195" s="5"/>
@@ -66656,15 +66830,15 @@
     </row>
     <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G282" s="0" t="s">
-        <v>193</v>
+        <v>206</v>
       </c>
       <c r="H282" s="0" t="s">
-        <v>194</v>
+        <v>207</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C283" s="0" t="s">
-        <v>195</v>
+        <v>208</v>
       </c>
       <c r="F283" s="0" t="n">
         <v>2020</v>
@@ -66691,7 +66865,7 @@
         <v>0.275162857371758</v>
       </c>
       <c r="J284" s="0" t="s">
-        <v>196</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>